<commit_message>
EPBDS-7428	Support transposed Simple rules and Smart rules
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-6161_ShouldNotCast.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-6161_ShouldNotCast.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C1A1EEA-03C0-4BC3-909A-91E84500ED4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="11685"/>
+    <workbookView xWindow="1395" yWindow="180" windowWidth="26505" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="7" r:id="rId1"/>
@@ -20,12 +21,36 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Автор</author>
   </authors>
   <commentList>
-    <comment ref="B26" authorId="0" shapeId="0">
+    <comment ref="B26" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Автор:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Тест кейс должен падать. Т.к. не возможно закастить Object[] или String к List</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C26" authorId="0" shapeId="0" xr:uid="{51966330-A650-4BBA-B6C5-F1B17B4C7699}">
       <text>
         <r>
           <rPr>
@@ -54,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>RETURN</t>
   </si>
@@ -62,13 +87,16 @@
     <t>One, Two, Three</t>
   </si>
   <si>
-    <t>SimpleRules List SomeLogic()</t>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>SimpleRules List SomeLogic(Integer value)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="8">
     <font>
       <sz val="11"/>
@@ -208,8 +236,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="20% - Accent1 10" xfId="2"/>
-    <cellStyle name="20% - Accent1 2" xfId="1"/>
+    <cellStyle name="20% - Accent1 10" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="20% - Accent1 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -237,7 +265,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -270,7 +298,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -402,6 +436,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -437,6 +488,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -612,11 +680,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B24:B26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B24:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C32" sqref="C32:C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -628,21 +696,28 @@
     <col min="5" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="24" spans="2:2">
+    <row r="24" spans="2:3">
       <c r="B24" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B25" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="2:2">
-      <c r="B25" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:2">
-      <c r="B26" s="3" t="s">
+    <row r="26" spans="2:3" ht="16.5" thickTop="1" thickBot="1">
+      <c r="B26" s="3">
+        <v>1</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>1</v>
       </c>
     </row>
+    <row r="27" spans="2:3" ht="15.75" thickTop="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>